<commit_message>
docs(diseño): Actualiza Estados, Responsables y Estados de Prueba en PB
</commit_message>
<xml_diff>
--- a/02 DESARROLLO/SCELS/02 DISEÑO/SCELS-PB-009.xlsx
+++ b/02 DESARROLLO/SCELS/02 DISEÑO/SCELS-PB-009.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ciclo 2022\2022-1\BAKATI 2\BAKATI-GROUP\02 DESARROLLO\SCELS\02 DISEÑO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Ciclo 2022\2022-1\BAKATI 3\BAKATI-GROUP\02 DESARROLLO\SCELS\02 DISEÑO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A62AECC-167C-4B64-9CB2-DAAE4B73B7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C4BE830-95FB-481A-B000-5B3FF5757CDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="945" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRODUCT BACKLOG" sheetId="1" r:id="rId1"/>
@@ -184,9 +184,6 @@
     <t>ADMINISTRADOR</t>
   </si>
   <si>
-    <t>tener una gestión de categorías de productos</t>
-  </si>
-  <si>
     <t>poder clasificar los productos de mi tienda virtual en categorías</t>
   </si>
   <si>
@@ -194,9 +191,6 @@
   </si>
   <si>
     <t>AGREGAR MÓDULO PRODUCTOS EN ADMIN</t>
-  </si>
-  <si>
-    <t>tener una gestión de los productos de mi tienda</t>
   </si>
   <si>
     <t>poder controlar el inventario de mi tienda virtual</t>
@@ -502,6 +496,12 @@
     <t>Aracelli Zevallos
 Frank Jacobo
 Guillermo Savero</t>
+  </si>
+  <si>
+    <t>Tener una gestión de categorías de productos</t>
+  </si>
+  <si>
+    <t>Tener una gestión de los productos de mi tienda</t>
   </si>
 </sst>
 </file>
@@ -1287,7 +1287,7 @@
   <dimension ref="A1:AE1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1307,7 +1307,7 @@
     <col min="14" max="14" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="51.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1340,7 +1340,7 @@
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
     </row>
-    <row r="2" spans="1:31" ht="51.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="50" t="s">
         <v>0</v>
@@ -1716,10 +1716,10 @@
         <v>31</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>32</v>
+        <v>116</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="7">
         <v>1</v>
@@ -1729,16 +1729,16 @@
       </c>
       <c r="J11" s="15"/>
       <c r="K11" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O11" s="16"/>
       <c r="P11" s="16"/>
@@ -1761,22 +1761,22 @@
     <row r="12" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>36</v>
+        <v>117</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H12" s="7">
         <v>1</v>
@@ -1786,13 +1786,13 @@
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N12" s="15" t="s">
         <v>14</v>
@@ -1818,22 +1818,22 @@
     <row r="13" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H13" s="7">
         <v>2</v>
@@ -1843,13 +1843,13 @@
       </c>
       <c r="J13" s="15"/>
       <c r="K13" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L13" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N13" s="15" t="s">
         <v>7</v>
@@ -1875,22 +1875,22 @@
     <row r="14" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H14" s="7">
         <v>1</v>
@@ -1900,13 +1900,13 @@
       </c>
       <c r="J14" s="15"/>
       <c r="K14" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L14" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N14" s="15" t="s">
         <v>7</v>
@@ -1932,22 +1932,22 @@
     <row r="15" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H15" s="7">
         <v>2</v>
@@ -1957,13 +1957,13 @@
       </c>
       <c r="J15" s="15"/>
       <c r="K15" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N15" s="15" t="s">
         <v>14</v>
@@ -1989,22 +1989,22 @@
     <row r="16" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E16" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H16" s="7">
         <v>3</v>
@@ -2014,16 +2014,16 @@
       </c>
       <c r="J16" s="15"/>
       <c r="K16" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L16" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N16" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O16" s="16"/>
       <c r="P16" s="16"/>
@@ -2046,22 +2046,22 @@
     <row r="17" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="G17" s="15" t="s">
         <v>52</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="H17" s="7">
         <v>1</v>
@@ -2071,13 +2071,13 @@
       </c>
       <c r="J17" s="15"/>
       <c r="K17" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L17" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N17" s="15" t="s">
         <v>14</v>
@@ -2103,22 +2103,22 @@
     <row r="18" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H18" s="7">
         <v>2</v>
@@ -2128,16 +2128,16 @@
       </c>
       <c r="J18" s="15"/>
       <c r="K18" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L18" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N18" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O18" s="16"/>
       <c r="P18" s="16"/>
@@ -2160,22 +2160,22 @@
     <row r="19" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H19" s="7">
         <v>2</v>
@@ -2185,13 +2185,13 @@
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L19" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N19" s="15" t="s">
         <v>7</v>
@@ -2217,22 +2217,22 @@
     <row r="20" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H20" s="7">
         <v>3</v>
@@ -2242,13 +2242,13 @@
       </c>
       <c r="J20" s="15"/>
       <c r="K20" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L20" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N20" s="15" t="s">
         <v>7</v>
@@ -2274,22 +2274,22 @@
     <row r="21" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H21" s="7">
         <v>3</v>
@@ -2299,16 +2299,16 @@
       </c>
       <c r="J21" s="15"/>
       <c r="K21" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L21" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M21" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N21" s="15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O21" s="16"/>
       <c r="P21" s="16"/>
@@ -2331,22 +2331,22 @@
     <row r="22" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G22" s="15" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H22" s="7">
         <v>3</v>
@@ -2356,13 +2356,13 @@
       </c>
       <c r="J22" s="15"/>
       <c r="K22" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L22" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N22" s="15" t="s">
         <v>14</v>
@@ -2388,22 +2388,22 @@
     <row r="23" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H23" s="7">
         <v>2</v>
@@ -2413,13 +2413,13 @@
       </c>
       <c r="J23" s="15"/>
       <c r="K23" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L23" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N23" s="15" t="s">
         <v>14</v>
@@ -2445,22 +2445,22 @@
     <row r="24" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H24" s="7">
         <v>2</v>
@@ -2470,13 +2470,13 @@
       </c>
       <c r="J24" s="15"/>
       <c r="K24" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N24" s="15" t="s">
         <v>7</v>
@@ -34815,7 +34815,7 @@
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="57" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="51"/>
       <c r="C1" s="51"/>
@@ -34875,27 +34875,27 @@
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="59"/>
       <c r="D3" s="59"/>
       <c r="E3" s="60"/>
       <c r="F3" s="19"/>
       <c r="G3" s="20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H3" s="20" t="s">
         <v>2</v>
       </c>
       <c r="I3" s="19"/>
       <c r="J3" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
@@ -34922,17 +34922,17 @@
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="23" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H4" s="24">
         <v>1</v>
       </c>
       <c r="I4" s="22"/>
       <c r="J4" s="25" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K4" s="26" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
@@ -34953,13 +34953,13 @@
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="28">
         <v>44706</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="30">
         <v>44652</v>
@@ -34967,17 +34967,17 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="23" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H5" s="24">
         <v>2</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K5" s="26" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
@@ -35004,7 +35004,7 @@
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="23" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H6" s="24">
         <v>3</v>
@@ -35069,25 +35069,25 @@
         <v>18</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E8" s="36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G8" s="35" t="s">
         <v>1</v>
       </c>
       <c r="H8" s="35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I8" s="35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K8" s="35" t="s">
         <v>24</v>
@@ -35113,7 +35113,7 @@
     </row>
     <row r="9" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B9" s="37"/>
       <c r="C9" s="38"/>
@@ -35144,7 +35144,7 @@
     </row>
     <row r="10" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="38"/>
@@ -36282,13 +36282,13 @@
       <c r="D49" s="17"/>
       <c r="E49" s="40"/>
       <c r="F49" s="40" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G49" s="40" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H49" s="40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I49" s="17"/>
       <c r="J49" s="17"/>
@@ -36316,7 +36316,7 @@
       <c r="C50" s="17"/>
       <c r="D50" s="40"/>
       <c r="E50" s="40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F50" s="40">
         <v>20</v>
@@ -36353,7 +36353,7 @@
       <c r="C51" s="17"/>
       <c r="D51" s="40"/>
       <c r="E51" s="40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F51" s="40"/>
       <c r="G51" s="40"/>
@@ -36386,7 +36386,7 @@
       <c r="C52" s="17"/>
       <c r="D52" s="40"/>
       <c r="E52" s="40" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F52" s="40">
         <v>20</v>
@@ -36395,7 +36395,7 @@
         <v>12</v>
       </c>
       <c r="H52" s="40" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I52" s="17"/>
       <c r="J52" s="17"/>

</xml_diff>